<commit_message>
ATA da reunião do dia 06/04/2020
</commit_message>
<xml_diff>
--- a/documentação/ATA-Projeto 2.0.xlsx
+++ b/documentação/ATA-Projeto 2.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Presentes</t>
   </si>
@@ -45,6 +45,30 @@
   </si>
   <si>
     <t>ATA - Projeto 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1 -  Product Owner: Gabriel</t>
+  </si>
+  <si>
+    <t>5 - CSS do site institucional</t>
+  </si>
+  <si>
+    <t>Raphael Moitinho, Stefany Batista, Graziela, Gabriel Bezerra, Yuri Vedovate, Bruno Santana</t>
+  </si>
+  <si>
+    <t>2 - Definição do que será feito essa semana</t>
+  </si>
+  <si>
+    <t>3 - Fazer prototipo do site</t>
+  </si>
+  <si>
+    <t>4 - Marcar como feita as atividades</t>
+  </si>
+  <si>
+    <t>6 - Ver o que é dashboard com yoshi</t>
   </si>
 </sst>
 </file>
@@ -140,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -163,35 +187,17 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-0.749992370372631"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -393,13 +399,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -412,6 +411,37 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-0.749992370372631"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -427,18 +457,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A11:F18" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A11:F18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A11:F18"/>
   <sortState ref="A12:F18">
     <sortCondition ref="D1:D8"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="4" name="Data" dataDxfId="6"/>
-    <tableColumn id="6" name="Horário de início" dataDxfId="5"/>
-    <tableColumn id="7" name="Horário de Término" dataDxfId="4"/>
-    <tableColumn id="5" name="Presentes" dataDxfId="3"/>
-    <tableColumn id="3" name="Ausentes" dataDxfId="2"/>
-    <tableColumn id="8" name="Assuntos em pauta" dataDxfId="1"/>
+    <tableColumn id="4" name="Data" dataDxfId="5"/>
+    <tableColumn id="6" name="Horário de início" dataDxfId="4"/>
+    <tableColumn id="7" name="Horário de Término" dataDxfId="3"/>
+    <tableColumn id="5" name="Presentes" dataDxfId="2"/>
+    <tableColumn id="3" name="Ausentes" dataDxfId="1"/>
+    <tableColumn id="8" name="Assuntos em pauta" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -709,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -777,55 +807,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="1"/>
+    <row r="12" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>43927</v>
+      </c>
+      <c r="B12" s="9">
+        <v>0.79375000000000007</v>
+      </c>
+      <c r="C12" s="9">
+        <v>0.81736111111111109</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F12" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>

</xml_diff>

<commit_message>
ATA da reunião do dia 08/04/2020
</commit_message>
<xml_diff>
--- a/documentação/ATA-Projeto 2.0.xlsx
+++ b/documentação/ATA-Projeto 2.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Presentes</t>
   </si>
@@ -50,25 +50,19 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>1 -  Product Owner: Gabriel</t>
-  </si>
-  <si>
-    <t>5 - CSS do site institucional</t>
-  </si>
-  <si>
     <t>Raphael Moitinho, Stefany Batista, Graziela, Gabriel Bezerra, Yuri Vedovate, Bruno Santana</t>
   </si>
   <si>
-    <t>2 - Definição do que será feito essa semana</t>
-  </si>
-  <si>
-    <t>3 - Fazer prototipo do site</t>
-  </si>
-  <si>
-    <t>4 - Marcar como feita as atividades</t>
-  </si>
-  <si>
-    <t>6 - Ver o que é dashboard com yoshi</t>
+    <t>Raphael Moitinho, Stefany Batista, Gabriel Bezerra, Yuri Vedovate, Bruno Santana</t>
+  </si>
+  <si>
+    <t>1 -  Product Owner: Gabriel   2 - Definição do que será feito essa semana                  3 - Fazer prototipo do site       4 - Marcar como feita as atividades                                   5 - CSS do site institucional   6 - Ver o que é dashboard com yoshi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - o que será falado com o branão                                       2 - Pesquisar sobre o que é dashboard (informar dados de qual lugar tem mais lixo. EX: mais lixo na região norte)                                                                              3 - houve atualização do LLD e no HLD                                        4- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">graziela </t>
   </si>
 </sst>
 </file>
@@ -184,14 +178,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,38 +748,38 @@
   <sheetData>
     <row r="1" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" ht="0.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -807,31 +801,39 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+    <row r="12" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>43927</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>0.79375000000000007</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>0.81736111111111109</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>43929</v>
+      </c>
+      <c r="B13" s="8">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.8125</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="E13" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>11</v>
@@ -845,19 +847,15 @@
       <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -865,9 +863,7 @@
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -875,9 +871,7 @@
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>

</xml_diff>

<commit_message>
ATA da Reunião do dia 13/04/2020
</commit_message>
<xml_diff>
--- a/documentação/ATA-Projeto 2.0.xlsx
+++ b/documentação/ATA-Projeto 2.0.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Presentes</t>
   </si>
@@ -63,6 +64,9 @@
   </si>
   <si>
     <t xml:space="preserve">graziela </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 -  dashboard: separado por equipes para mostrar até quarta feira para o grupo;                                           2 - reunião com o grupo sobre arduino e banco de dados quinta feira depois da aula;                                            </t>
   </si>
 </sst>
 </file>
@@ -733,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +823,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43929</v>
       </c>
@@ -839,15 +843,25 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+    <row r="14" spans="1:6" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>43934</v>
+      </c>
+      <c r="B14" s="8">
+        <v>0.78541666666666676</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -891,4 +905,18 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
ATA do dia 15/04/2020
</commit_message>
<xml_diff>
--- a/documentação/ATA-Projeto 2.0.xlsx
+++ b/documentação/ATA-Projeto 2.0.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Presentes</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t xml:space="preserve">1 -  dashboard: separado por equipes para mostrar até quarta feira para o grupo;                                           2 - reunião com o grupo sobre arduino e banco de dados quinta feira depois da aula;                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stefany Batista, Graziela, Gabriel Bezerra, Yuri Vedovate, Bruno Santana, Raphael Moitinho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 -  começamos falando sobre ideias de dashboard.            2 - decisão para saber quais as melhores informações para colocarmos no nosso dashboard.                                3 -  não conseguimos decidir qual o melhor dashboard, então decidimos entrar em contato com alguém que tenha mais experiência no assunto, no caso o Thiago.                                      </t>
   </si>
 </sst>
 </file>
@@ -737,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="D14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,13 +869,23 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+    <row r="15" spans="1:6" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>43936</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.84652777777777777</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>

</xml_diff>

<commit_message>
ATA da reunião do dia 20/04/2020
</commit_message>
<xml_diff>
--- a/documentação/ATA-Projeto 2.0.xlsx
+++ b/documentação/ATA-Projeto 2.0.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Presentes</t>
   </si>
@@ -73,6 +72,15 @@
   </si>
   <si>
     <t xml:space="preserve">1 -  começamos falando sobre ideias de dashboard.            2 - decisão para saber quais as melhores informações para colocarmos no nosso dashboard.                                3 -  não conseguimos decidir qual o melhor dashboard, então decidimos entrar em contato com alguém que tenha mais experiência no assunto, no caso o Thiago.                                      </t>
+  </si>
+  <si>
+    <t>20/042020</t>
+  </si>
+  <si>
+    <t>Stefany Batista, Graziela, Gabriel Bezerra, Yuri Vedovate, Bruno Santana, Raphael Moitinho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 - o que fazer essa semana   2 - focar nas atividades de cada dupla.                               3 - quinta feira (23/04/2020) ensaio geral para as apresentações.                                   </t>
   </si>
 </sst>
 </file>
@@ -743,8 +751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,7 +877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>43936</v>
       </c>
@@ -887,13 +895,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+    <row r="16" spans="1:6" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="C16" s="8">
+        <v>0.80069444444444438</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="17" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
@@ -921,18 +939,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
ATA da reunião do dia 22/04/2020
</commit_message>
<xml_diff>
--- a/documentação/ATA-Projeto 2.0.xlsx
+++ b/documentação/ATA-Projeto 2.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Presentes</t>
   </si>
@@ -81,13 +81,19 @@
   </si>
   <si>
     <t xml:space="preserve">1 - o que fazer essa semana   2 - focar nas atividades de cada dupla.                               3 - quinta feira (23/04/2020) ensaio geral para as apresentações.                                   </t>
+  </si>
+  <si>
+    <t>Stefany Batista, Graziela, Gabriel Bezerra, Yuri Vedovate, Bruno Santana, Raphael Moitinho.</t>
+  </si>
+  <si>
+    <t>1 - como será feito o dashboard.                                        2 -  separação das duplas para que cada um faça o seu próprio protótipo de dashboard                                 3 - ensaio de amanhã cancelado por motivos de sobrecarga com conteúdos. Ensaio marcado para domingo dia 22/042020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +131,13 @@
       <b/>
       <sz val="28"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -176,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -204,6 +217,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,18 +929,28 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+    <row r="17" spans="1:6" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>43943</v>
+      </c>
+      <c r="B17" s="8">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="C17" s="8">
+        <v>0.82916666666666661</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>

</xml_diff>